<commit_message>
Ajout de bibliothèque JS
</commit_message>
<xml_diff>
--- a/data/capacites.xlsx
+++ b/data/capacites.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -650,12 +650,15 @@
   <dimension ref="A1:BI14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="BB20" sqref="BB20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -840,7 +843,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -1025,7 +1028,7 @@
         <v>26681</v>
       </c>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1051,166 +1054,166 @@
         <v>75753</v>
       </c>
       <c r="I3">
-        <v>404934</v>
+        <v>202467</v>
       </c>
       <c r="J3">
-        <v>211294</v>
+        <v>105647</v>
       </c>
       <c r="K3">
-        <v>226874</v>
+        <v>113437</v>
       </c>
       <c r="L3">
-        <v>210652</v>
+        <v>105326</v>
       </c>
       <c r="M3">
-        <v>217562</v>
+        <v>108781</v>
       </c>
       <c r="N3">
-        <v>246342</v>
+        <v>123171</v>
       </c>
       <c r="O3">
-        <v>328768</v>
+        <v>164384</v>
       </c>
       <c r="P3">
-        <v>370280</v>
+        <v>185140</v>
       </c>
       <c r="Q3">
-        <v>358966</v>
+        <v>179483</v>
       </c>
       <c r="R3">
-        <v>339390</v>
+        <v>169695</v>
       </c>
       <c r="S3">
-        <v>265134</v>
+        <v>132567</v>
       </c>
       <c r="T3">
-        <v>370734</v>
+        <v>185367</v>
       </c>
       <c r="U3">
-        <v>606788</v>
+        <v>303394</v>
       </c>
       <c r="V3">
-        <v>478578</v>
+        <v>239289</v>
       </c>
       <c r="W3">
-        <v>479490</v>
+        <v>239745</v>
       </c>
       <c r="X3">
-        <v>598172</v>
+        <v>299086</v>
       </c>
       <c r="Y3">
-        <v>488594</v>
+        <v>244297</v>
       </c>
       <c r="Z3">
-        <v>594880</v>
+        <v>297440</v>
       </c>
       <c r="AA3">
-        <v>742926</v>
+        <v>371463</v>
       </c>
       <c r="AB3">
-        <v>482002</v>
+        <v>241001</v>
       </c>
       <c r="AC3">
-        <v>323384</v>
+        <v>161692</v>
       </c>
       <c r="AD3">
-        <v>577378</v>
+        <v>288689</v>
       </c>
       <c r="AE3">
-        <v>590020</v>
+        <v>295010</v>
       </c>
       <c r="AF3">
-        <v>677292</v>
+        <v>338646</v>
       </c>
       <c r="AG3">
-        <v>715382</v>
+        <v>357691</v>
       </c>
       <c r="AH3">
-        <v>838156</v>
+        <v>419078</v>
       </c>
       <c r="AI3">
-        <v>961652</v>
+        <v>480826</v>
       </c>
       <c r="AJ3">
-        <v>1273646</v>
+        <v>636823</v>
       </c>
       <c r="AK3">
-        <v>1409688</v>
+        <v>704844</v>
       </c>
       <c r="AL3">
-        <v>1519818</v>
+        <v>759909</v>
       </c>
       <c r="AM3">
-        <v>1523460</v>
+        <v>761730</v>
       </c>
       <c r="AN3">
-        <v>1673388</v>
+        <v>836694</v>
       </c>
       <c r="AO3">
-        <v>1781104</v>
+        <v>890552</v>
       </c>
       <c r="AP3">
-        <v>1430518</v>
+        <v>715259</v>
       </c>
       <c r="AQ3">
-        <v>849162</v>
+        <v>424581</v>
       </c>
       <c r="AR3">
-        <v>786984</v>
+        <v>393492</v>
       </c>
       <c r="AS3">
-        <v>831174</v>
+        <v>415587</v>
       </c>
       <c r="AT3">
-        <v>741642</v>
+        <v>370821</v>
       </c>
       <c r="AU3">
-        <v>594876</v>
+        <v>297438</v>
       </c>
       <c r="AV3">
-        <v>518134</v>
+        <v>259067</v>
       </c>
       <c r="AW3">
-        <v>496624</v>
+        <v>248312</v>
       </c>
       <c r="AX3">
-        <v>448602</v>
+        <v>224301</v>
       </c>
       <c r="AY3">
-        <v>524734</v>
+        <v>262367</v>
       </c>
       <c r="AZ3">
-        <v>518538</v>
+        <v>259269</v>
       </c>
       <c r="BA3">
-        <v>325552</v>
+        <v>162776</v>
       </c>
       <c r="BB3">
-        <v>289964</v>
+        <v>144982</v>
       </c>
       <c r="BC3">
-        <v>288632</v>
+        <v>144316</v>
       </c>
       <c r="BD3">
-        <v>251056</v>
+        <v>125528</v>
       </c>
       <c r="BE3">
-        <v>239762</v>
+        <v>119881</v>
       </c>
       <c r="BF3">
-        <v>228266</v>
+        <v>114133</v>
       </c>
       <c r="BG3">
-        <v>334552</v>
+        <v>167276</v>
       </c>
       <c r="BH3">
-        <v>616942</v>
+        <v>308471</v>
       </c>
       <c r="BI3">
-        <v>98964</v>
+        <v>49482</v>
       </c>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1395,7 +1398,7 @@
         <v>29585</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -1580,7 +1583,7 @@
         <v>77267</v>
       </c>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -1765,7 +1768,7 @@
         <v>137257</v>
       </c>
     </row>
-    <row r="7" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -1950,7 +1953,7 @@
         <v>22162</v>
       </c>
     </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -2135,7 +2138,7 @@
         <v>153813</v>
       </c>
     </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -2320,7 +2323,7 @@
         <v>29453</v>
       </c>
     </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -2505,7 +2508,7 @@
         <v>12634</v>
       </c>
     </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -2690,7 +2693,7 @@
         <v>71178</v>
       </c>
     </row>
-    <row r="12" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -2875,7 +2878,7 @@
         <v>131465</v>
       </c>
     </row>
-    <row r="13" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -3060,7 +3063,7 @@
         <v>29471</v>
       </c>
     </row>
-    <row r="14" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>73</v>
       </c>

</xml_diff>